<commit_message>
After summer 2021 commit. Various fixes, notably groupings.
</commit_message>
<xml_diff>
--- a/filelist.xlsx
+++ b/filelist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baim/IMR/2021-biotic/bess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69774656-E689-984C-8411-9A9978745C19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7B231C-4D40-314F-8E0A-A14190E4A8B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="17640" xr2:uid="{E7D8AA63-0CDF-4928-AADB-C8AE34FFBE75}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
   <si>
     <t>År</t>
   </si>
@@ -499,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CC5254-39A1-4C89-A39D-975A471D583D}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -539,10 +539,10 @@
         <v>2003</v>
       </c>
       <c r="B3">
-        <v>2003703</v>
+        <v>2003209</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -550,21 +550,21 @@
         <v>2003</v>
       </c>
       <c r="B4">
-        <v>2003209</v>
+        <v>2003110</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2003</v>
       </c>
-      <c r="B5">
-        <v>2003110</v>
+      <c r="B5" t="s">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -572,21 +572,21 @@
         <v>2003</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2003</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
+        <v>2004</v>
+      </c>
+      <c r="B7">
+        <v>2004702</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -594,54 +594,54 @@
         <v>2004</v>
       </c>
       <c r="B8">
-        <v>2004703</v>
+        <v>2004210</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2004</v>
       </c>
-      <c r="B9">
-        <v>2004702</v>
+      <c r="B9" t="s">
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2004</v>
       </c>
-      <c r="B10">
-        <v>2004210</v>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2004</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
+        <v>2005</v>
+      </c>
+      <c r="B11">
+        <v>2005703</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2004</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
+        <v>2005</v>
+      </c>
+      <c r="B12">
+        <v>2005702</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -649,10 +649,10 @@
         <v>2005</v>
       </c>
       <c r="B13">
-        <v>2005703</v>
+        <v>2005209</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -660,54 +660,54 @@
         <v>2005</v>
       </c>
       <c r="B14">
-        <v>2005702</v>
+        <v>2005111</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2005</v>
       </c>
-      <c r="B15">
-        <v>2005209</v>
+      <c r="B15" t="s">
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2005</v>
       </c>
-      <c r="B16">
-        <v>2005111</v>
+      <c r="B16" t="s">
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2005</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
+        <v>2006</v>
+      </c>
+      <c r="B17">
+        <v>2006704</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2005</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
+        <v>2006</v>
+      </c>
+      <c r="B18">
+        <v>2006702</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -715,10 +715,10 @@
         <v>2006</v>
       </c>
       <c r="B19">
-        <v>2006704</v>
+        <v>2006211</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -726,54 +726,54 @@
         <v>2006</v>
       </c>
       <c r="B20">
-        <v>2006702</v>
+        <v>2006113</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2006</v>
       </c>
-      <c r="B21">
-        <v>2006211</v>
+      <c r="B21" t="s">
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2006</v>
       </c>
-      <c r="B22">
-        <v>2006113</v>
+      <c r="B22" t="s">
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2006</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
+        <v>2007</v>
+      </c>
+      <c r="B23">
+        <v>2007702</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2006</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
+        <v>2007</v>
+      </c>
+      <c r="B24">
+        <v>2007210</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -781,54 +781,54 @@
         <v>2007</v>
       </c>
       <c r="B25">
-        <v>2007702</v>
+        <v>2007110</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2007</v>
       </c>
-      <c r="B26">
-        <v>2007210</v>
+      <c r="B26" t="s">
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2007</v>
       </c>
-      <c r="B27">
-        <v>2007110</v>
+      <c r="B27" t="s">
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2007</v>
-      </c>
-      <c r="B28" t="s">
-        <v>16</v>
+        <v>2008</v>
+      </c>
+      <c r="B28">
+        <v>2008822</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2007</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
+        <v>2008</v>
+      </c>
+      <c r="B29">
+        <v>2008703</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -836,10 +836,10 @@
         <v>2008</v>
       </c>
       <c r="B30">
-        <v>2008822</v>
+        <v>2008208</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -847,43 +847,43 @@
         <v>2008</v>
       </c>
       <c r="B31">
-        <v>2008703</v>
+        <v>2008106</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2008</v>
       </c>
-      <c r="B32">
-        <v>2008208</v>
+      <c r="B32" t="s">
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B33">
-        <v>2008106</v>
+        <v>2009702</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2008</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
+        <v>2009</v>
+      </c>
+      <c r="B34">
+        <v>2009208</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -891,43 +891,43 @@
         <v>2009</v>
       </c>
       <c r="B35">
-        <v>2009702</v>
+        <v>2009109</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2009</v>
       </c>
-      <c r="B36">
-        <v>2009208</v>
+      <c r="B36" t="s">
+        <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B37">
-        <v>2009109</v>
+        <v>2010703</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2009</v>
-      </c>
-      <c r="B38" t="s">
-        <v>20</v>
+        <v>2010</v>
+      </c>
+      <c r="B38">
+        <v>2010210</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -935,54 +935,54 @@
         <v>2010</v>
       </c>
       <c r="B39">
-        <v>2010703</v>
+        <v>2010111</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2010</v>
       </c>
-      <c r="B40">
-        <v>2010210</v>
+      <c r="B40" t="s">
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2010</v>
       </c>
-      <c r="B41">
-        <v>2010111</v>
+      <c r="B41" t="s">
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>2010</v>
-      </c>
-      <c r="B42" t="s">
-        <v>21</v>
+        <v>2011</v>
+      </c>
+      <c r="B42">
+        <v>2011830</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>2010</v>
-      </c>
-      <c r="B43" t="s">
-        <v>22</v>
+        <v>2011</v>
+      </c>
+      <c r="B43">
+        <v>2011717</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -990,43 +990,43 @@
         <v>2011</v>
       </c>
       <c r="B44">
-        <v>2011830</v>
+        <v>2011213</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2011</v>
       </c>
-      <c r="B45">
-        <v>2011717</v>
+      <c r="B45" t="s">
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B46">
-        <v>2011213</v>
+        <v>2012845</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>2011</v>
-      </c>
-      <c r="B47" t="s">
-        <v>23</v>
+        <v>2012</v>
+      </c>
+      <c r="B47">
+        <v>2012209</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1034,43 +1034,43 @@
         <v>2012</v>
       </c>
       <c r="B48">
-        <v>2012845</v>
+        <v>2012111</v>
       </c>
       <c r="C48" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2012</v>
       </c>
-      <c r="B49">
-        <v>2012209</v>
+      <c r="B49" t="s">
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B50">
-        <v>2012111</v>
+        <v>2013843</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>2012</v>
-      </c>
-      <c r="B51" t="s">
-        <v>26</v>
+        <v>2013</v>
+      </c>
+      <c r="B51">
+        <v>2013208</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -1078,43 +1078,43 @@
         <v>2013</v>
       </c>
       <c r="B52">
-        <v>2013843</v>
+        <v>2013111</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2013</v>
       </c>
-      <c r="B53">
-        <v>2013208</v>
+      <c r="B53" t="s">
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B54">
-        <v>2013111</v>
+        <v>2014806</v>
       </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>2013</v>
-      </c>
-      <c r="B55" t="s">
-        <v>27</v>
+        <v>2014</v>
+      </c>
+      <c r="B55">
+        <v>2014212</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1122,43 +1122,43 @@
         <v>2014</v>
       </c>
       <c r="B56">
-        <v>2014806</v>
+        <v>2014116</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2014</v>
       </c>
-      <c r="B57">
-        <v>2014212</v>
+      <c r="B57" t="s">
+        <v>28</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B58">
-        <v>2014116</v>
+        <v>2015843</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>2014</v>
-      </c>
-      <c r="B59" t="s">
-        <v>28</v>
+        <v>2015</v>
+      </c>
+      <c r="B59">
+        <v>2015210</v>
       </c>
       <c r="C59" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -1166,43 +1166,43 @@
         <v>2015</v>
       </c>
       <c r="B60">
-        <v>2015843</v>
+        <v>2015114</v>
       </c>
       <c r="C60" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2015</v>
       </c>
-      <c r="B61">
-        <v>2015210</v>
+      <c r="B61" t="s">
+        <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B62">
-        <v>2015114</v>
+        <v>2016847</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>2015</v>
-      </c>
-      <c r="B63" t="s">
-        <v>29</v>
+        <v>2016</v>
+      </c>
+      <c r="B63">
+        <v>2016842</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -1210,43 +1210,43 @@
         <v>2016</v>
       </c>
       <c r="B64">
-        <v>2016847</v>
+        <v>2016209</v>
       </c>
       <c r="C64" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2016</v>
       </c>
-      <c r="B65">
-        <v>2016842</v>
+      <c r="B65" t="s">
+        <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B66">
-        <v>2016209</v>
+        <v>2017856</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>2016</v>
-      </c>
-      <c r="B67" t="s">
-        <v>30</v>
+        <v>2017</v>
+      </c>
+      <c r="B67">
+        <v>2017209</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
@@ -1254,43 +1254,43 @@
         <v>2017</v>
       </c>
       <c r="B68">
-        <v>2017856</v>
+        <v>2017113</v>
       </c>
       <c r="C68" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2017</v>
       </c>
-      <c r="B69">
-        <v>2017209</v>
+      <c r="B69" t="s">
+        <v>32</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B70">
-        <v>2017113</v>
+        <v>2018838</v>
       </c>
       <c r="C70" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>2017</v>
-      </c>
-      <c r="B71" t="s">
-        <v>32</v>
+        <v>2018</v>
+      </c>
+      <c r="B71">
+        <v>2018209</v>
       </c>
       <c r="C71" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
@@ -1298,43 +1298,43 @@
         <v>2018</v>
       </c>
       <c r="B72">
-        <v>2018838</v>
+        <v>2018110</v>
       </c>
       <c r="C72" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2018</v>
       </c>
-      <c r="B73">
-        <v>2018209</v>
+      <c r="B73" t="s">
+        <v>33</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B74">
-        <v>2018110</v>
+        <v>2019813</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>2018</v>
-      </c>
-      <c r="B75" t="s">
-        <v>33</v>
+        <v>2019</v>
+      </c>
+      <c r="B75">
+        <v>2019209</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
@@ -1342,43 +1342,43 @@
         <v>2019</v>
       </c>
       <c r="B76">
-        <v>2019813</v>
+        <v>2019113</v>
       </c>
       <c r="C76" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2019</v>
       </c>
-      <c r="B77">
-        <v>2019209</v>
+      <c r="B77" t="s">
+        <v>34</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B78">
-        <v>2019113</v>
+        <v>2020706</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>2019</v>
-      </c>
-      <c r="B79" t="s">
-        <v>34</v>
+        <v>2020</v>
+      </c>
+      <c r="B79">
+        <v>2020209</v>
       </c>
       <c r="C79" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1386,53 +1386,31 @@
         <v>2020</v>
       </c>
       <c r="B80">
-        <v>2020706</v>
+        <v>2020111</v>
       </c>
       <c r="C80" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2020</v>
       </c>
-      <c r="B81">
-        <v>2020209</v>
+      <c r="B81" t="s">
+        <v>35</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2020</v>
       </c>
-      <c r="B82">
-        <v>2020111</v>
+      <c r="B82" t="s">
+        <v>40</v>
       </c>
       <c r="C82" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>2020</v>
-      </c>
-      <c r="B83" t="s">
-        <v>35</v>
-      </c>
-      <c r="C83" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>2020</v>
-      </c>
-      <c r="B84" t="s">
-        <v>40</v>
-      </c>
-      <c r="C84" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>